<commit_message>
add rule P/F detail in View
</commit_message>
<xml_diff>
--- a/Graduation2/wwwroot/template_2016CSE.xlsx
+++ b/Graduation2/wwwroot/template_2016CSE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/GraduationAssessment/GraduationAssesment/TestProject/TestProject/wwwroot/upload/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A0BF68-1030-4245-807F-86836C6663C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A960304-525D-4F46-85D4-1FC698EA435C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1266,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1314,7 +1314,7 @@
       <c r="D2" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1328,7 +1328,7 @@
       <c r="D3" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1342,7 +1342,7 @@
       <c r="D4" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
       <c r="D5" s="18">
         <v>2016</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1370,7 +1370,7 @@
       <c r="D6" s="18">
         <v>2016</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1387,11 +1387,11 @@
       <c r="D7" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" t="s">
         <v>91</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>101</v>
       </c>
       <c r="G7" t="s">
         <v>110</v>
@@ -1407,11 +1407,11 @@
       <c r="D8" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" t="s">
         <v>91</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1424,11 +1424,11 @@
       <c r="D9" s="17">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" t="s">
         <v>25</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1441,11 +1441,11 @@
       <c r="D10" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" t="s">
         <v>91</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1458,11 +1458,11 @@
       <c r="D11" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" t="s">
         <v>91</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1475,11 +1475,11 @@
       <c r="D12" s="17">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" t="s">
         <v>25</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1492,11 +1492,11 @@
       <c r="D13" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
         <v>91</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1509,11 +1509,11 @@
       <c r="D14" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" t="s">
         <v>91</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1526,11 +1526,11 @@
       <c r="D15" s="17">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="G15" t="s">
         <v>109</v>
@@ -1546,11 +1546,11 @@
       <c r="D16" s="17">
         <v>28</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" t="s">
         <v>25</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1566,11 +1566,11 @@
       <c r="D17" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" t="s">
         <v>92</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1583,11 +1583,11 @@
       <c r="D18" s="17">
         <v>42</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" t="s">
         <v>25</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1600,11 +1600,11 @@
       <c r="D19" s="17">
         <v>84</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="s">
         <v>25</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1617,11 +1617,11 @@
       <c r="D20" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" t="s">
         <v>94</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1634,11 +1634,11 @@
       <c r="D21" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" t="s">
         <v>94</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1651,11 +1651,11 @@
       <c r="D22" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" t="s">
         <v>94</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1668,11 +1668,11 @@
       <c r="D23" s="20">
         <v>6</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" t="s">
         <v>25</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1685,11 +1685,11 @@
       <c r="D24" s="20">
         <v>12</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" t="s">
         <v>25</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1705,11 +1705,11 @@
       <c r="D25" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" t="s">
         <v>95</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1722,11 +1722,11 @@
       <c r="D26" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" t="s">
         <v>95</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1739,11 +1739,11 @@
       <c r="D27" s="20">
         <v>2</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
         <v>39</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>57</v>
@@ -1759,11 +1759,11 @@
       <c r="D28" s="20">
         <v>4</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" t="s">
         <v>39</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -1777,11 +1777,11 @@
       <c r="D29" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" t="s">
         <v>95</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1794,11 +1794,11 @@
       <c r="D30" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" t="s">
         <v>95</v>
-      </c>
-      <c r="F30" s="24" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1811,11 +1811,11 @@
       <c r="D31" s="20">
         <v>140</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" t="s">
         <v>25</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="G31" t="s">
         <v>23</v>
@@ -1831,11 +1831,11 @@
       <c r="D32" s="20">
         <v>2</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
         <v>26</v>
-      </c>
-      <c r="F32" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
@@ -1854,11 +1854,11 @@
       <c r="D33" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="F33" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="48">
@@ -1871,11 +1871,11 @@
       <c r="D34" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1888,11 +1888,11 @@
       <c r="D35" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" t="s">
         <v>96</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1905,11 +1905,11 @@
       <c r="D36" s="20">
         <v>2</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s">
         <v>25</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1922,11 +1922,11 @@
       <c r="D37" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" t="s">
         <v>96</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>103</v>
       </c>
       <c r="G37" t="s">
         <v>45</v>
@@ -1942,11 +1942,11 @@
       <c r="D38" s="20">
         <v>0</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" t="s">
         <v>25</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1959,11 +1959,11 @@
       <c r="D39" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" t="s">
         <v>96</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>103</v>
       </c>
       <c r="G39" t="s">
         <v>46</v>
@@ -1979,11 +1979,11 @@
       <c r="D40" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" t="s">
         <v>92</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>101</v>
       </c>
       <c r="G40" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
bug fix, add bold text to FAIL rule
</commit_message>
<xml_diff>
--- a/Graduation2/wwwroot/template_2016CSE.xlsx
+++ b/Graduation2/wwwroot/template_2016CSE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/Graduation2/Graduation2/Graduation2/wwwroot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A960304-525D-4F46-85D4-1FC698EA435C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29999766-EE6F-F348-9FBA-4936922051D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="16900" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="전체질문목록" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="167">
   <si>
     <t>입력하려는 졸업기준의 학과(전공)명을 선택하세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -694,6 +694,14 @@
   </si>
   <si>
     <t>평점평균 기준을 입력하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE4074</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공개SW프로젝트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1266,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -2000,8 +2008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2075,11 +2083,21 @@
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2021</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">

</xml_diff>